<commit_message>
BE + FE Actors : fix actors without client handling (+ prevent CRA export if any not saved change)
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/CRA MONTH _COMPANY_ _DATE_.xlsx
+++ b/Ressources/DocTemplates/CRA MONTH _COMPANY_ _DATE_.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{671D62DB-641E-472C-8725-01D3D697A3BC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB319F0-17C7-4C0F-8745-5F236B42BB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="8940" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12300" yWindow="4755" windowWidth="37875" windowHeight="19875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRA" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>Client</t>
   </si>
@@ -79,6 +79,9 @@
   </si>
   <si>
     <t>Off</t>
+  </si>
+  <si>
+    <t>ActorId</t>
   </si>
 </sst>
 </file>
@@ -895,7 +898,7 @@
   <dimension ref="A1:AV266"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1143,6 +1146,9 @@
       <c r="AP8" t="s">
         <v>0</v>
       </c>
+      <c r="AQ8" t="s">
+        <v>15</v>
+      </c>
       <c r="AR8" s="34" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
BE ActorCRA : Add HR info and sort by company / name
</commit_message>
<xml_diff>
--- a/Ressources/DocTemplates/CRA MONTH _COMPANY_ _DATE_.xlsx
+++ b/Ressources/DocTemplates/CRA MONTH _COMPANY_ _DATE_.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Laurent\Golang\src\github.com\lpuig\ewin\doe\Ressources\DocTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB319F0-17C7-4C0F-8745-5F236B42BB5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D167A54-BFDF-4FFA-ADE1-6E97698C6F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12300" yWindow="4755" windowWidth="37875" windowHeight="19875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="30960" windowHeight="16920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CRA" sheetId="1" r:id="rId1"/>
+    <sheet name="Template" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">CRA!$1:$8</definedName>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
   <si>
     <t>Client</t>
   </si>
@@ -83,15 +84,31 @@
   <si>
     <t>ActorId</t>
   </si>
+  <si>
+    <t>Depl/j</t>
+  </si>
+  <si>
+    <t>Bonus Net</t>
+  </si>
+  <si>
+    <t>Salaire Net</t>
+  </si>
+  <si>
+    <t>Comment. Bonus</t>
+  </si>
+  <si>
+    <t>Groupe</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ [$€-40C]_-;\-* #,##0.00\ [$€-40C]_-;_-* &quot;-&quot;??\ [$€-40C]_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="mmmm\ yyyy"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="9" x14ac:knownFonts="1">
     <font>
@@ -413,7 +430,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -523,6 +540,8 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -897,8 +916,8 @@
   </sheetPr>
   <dimension ref="A1:AV266"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="AK1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AV14" sqref="AV14:AV15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -918,6 +937,11 @@
     <col min="14" max="35" width="3.7109375" customWidth="1"/>
     <col min="39" max="39" width="50.7109375" customWidth="1"/>
     <col min="40" max="40" width="4.28515625" customWidth="1"/>
+    <col min="42" max="42" width="20.7109375" customWidth="1"/>
+    <col min="43" max="43" width="12.42578125" customWidth="1"/>
+    <col min="44" max="46" width="12.7109375" style="39" customWidth="1"/>
+    <col min="47" max="47" width="20.7109375" style="40" customWidth="1"/>
+    <col min="48" max="48" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:48" x14ac:dyDescent="0.25">
@@ -960,33 +984,38 @@
       <c r="AO1" s="1"/>
       <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
+      <c r="AR1" s="1"/>
+      <c r="AS1" s="1"/>
+      <c r="AT1" s="1"/>
+      <c r="AU1" s="1"/>
+      <c r="AV1" s="1"/>
     </row>
     <row r="2" spans="2:48" x14ac:dyDescent="0.25">
       <c r="I2" s="8"/>
     </row>
     <row r="3" spans="2:48" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="41"/>
-      <c r="E3" s="47">
+      <c r="D3" s="43"/>
+      <c r="E3" s="49">
         <v>39448</v>
       </c>
-      <c r="F3" s="48"/>
-      <c r="G3" s="48"/>
-      <c r="H3" s="48"/>
-      <c r="I3" s="48"/>
-      <c r="J3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="51"/>
       <c r="K3"/>
       <c r="L3"/>
       <c r="M3"/>
     </row>
     <row r="7" spans="2:48" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="43"/>
-      <c r="D7" s="44"/>
+      <c r="C7" s="45"/>
+      <c r="D7" s="46"/>
       <c r="E7" s="15"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
@@ -1018,16 +1047,16 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="12"/>
       <c r="AI7" s="16"/>
-      <c r="AJ7" s="45" t="s">
+      <c r="AJ7" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="AK7" s="45" t="s">
+      <c r="AK7" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="AL7" s="45" t="s">
+      <c r="AL7" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="AM7" s="39" t="s">
+      <c r="AM7" s="41" t="s">
         <v>6</v>
       </c>
       <c r="AN7" s="11"/>
@@ -1135,34 +1164,34 @@
       <c r="AI8" s="22">
         <v>31</v>
       </c>
-      <c r="AJ8" s="46"/>
-      <c r="AK8" s="46"/>
-      <c r="AL8" s="46"/>
-      <c r="AM8" s="40"/>
+      <c r="AJ8" s="48"/>
+      <c r="AK8" s="48"/>
+      <c r="AL8" s="48"/>
+      <c r="AM8" s="42"/>
       <c r="AN8" s="11"/>
       <c r="AO8" t="s">
         <v>10</v>
       </c>
       <c r="AP8" t="s">
+        <v>20</v>
+      </c>
+      <c r="AQ8" t="s">
         <v>0</v>
       </c>
-      <c r="AQ8" t="s">
+      <c r="AR8" s="39" t="s">
+        <v>18</v>
+      </c>
+      <c r="AS8" s="39" t="s">
+        <v>16</v>
+      </c>
+      <c r="AT8" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="AU8" s="40" t="s">
+        <v>19</v>
+      </c>
+      <c r="AV8" t="s">
         <v>15</v>
-      </c>
-      <c r="AR8" s="34" t="s">
-        <v>11</v>
-      </c>
-      <c r="AS8" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT8" s="38" t="s">
-        <v>11</v>
-      </c>
-      <c r="AU8" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="AV8" s="37" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="9" spans="2:48" x14ac:dyDescent="0.25">
@@ -11499,4 +11528,36 @@
   <pageSetup paperSize="9" scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8361AD55-E651-436C-81A6-E9014ED286C9}">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="35" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="38" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="37" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>